<commit_message>
Jeg har tilføjet lidt mere data
</commit_message>
<xml_diff>
--- a/Testfil.xlsx
+++ b/Testfil.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B339958\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennislund/Documents/GitHub/Testrepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E018EC58-A69A-2B4C-9224-5381FD1DA425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,15 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Data</t>
   </si>
+  <si>
+    <t>Mere data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,23 +347,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
+      </c>
+      <c r="B2">
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jeg har tilføjet en tredje kolonne
</commit_message>
<xml_diff>
--- a/Testfil.xlsx
+++ b/Testfil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennislund/Documents/GitHub/Testrepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E018EC58-A69A-2B4C-9224-5381FD1DA425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391F594F-A4E8-1F48-990E-2214A9325613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Data</t>
   </si>
   <si>
     <t>Mere data</t>
+  </si>
+  <si>
+    <t>Og endnu mere</t>
   </si>
 </sst>
 </file>
@@ -348,28 +351,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
       <c r="B2">
         <v>456</v>
+      </c>
+      <c r="C2">
+        <v>789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Så har jeg lavet en selvstændig branch
</commit_message>
<xml_diff>
--- a/Testfil.xlsx
+++ b/Testfil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennislund/Documents/GitHub/Testrepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391F594F-A4E8-1F48-990E-2214A9325613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BA8DD6-A5A5-A647-A63F-E53FEF07D625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3160" yWindow="3760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Data</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Og endnu mere</t>
+  </si>
+  <si>
+    <t>Fjerde kolonne</t>
+  </si>
+  <si>
+    <t>Der bringer ændringer i sin egen branch</t>
   </si>
 </sst>
 </file>
@@ -351,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -369,8 +375,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
@@ -379,6 +388,9 @@
       </c>
       <c r="C2">
         <v>789</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jeg har tilføjet en lille kolonne efter den store
</commit_message>
<xml_diff>
--- a/Testfil.xlsx
+++ b/Testfil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennislund/Documents/GitHub/Testrepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391F594F-A4E8-1F48-990E-2214A9325613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2EC69A-70D8-7143-9F1D-44BC96FF711F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3160" yWindow="3760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Data</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Og endnu mere</t>
+  </si>
+  <si>
+    <t>Fjerde kolonne</t>
+  </si>
+  <si>
+    <t>Der bringer ændringer i sin egen branch</t>
   </si>
 </sst>
 </file>
@@ -351,15 +357,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -369,8 +378,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
@@ -379,6 +394,27 @@
       </c>
       <c r="C2">
         <v>789</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data2 kolonne tilføjet til regnearket
</commit_message>
<xml_diff>
--- a/Testfil.xlsx
+++ b/Testfil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennislund/Documents/GitHub/Testrepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2EC69A-70D8-7143-9F1D-44BC96FF711F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C43644-32DC-8948-89BB-6E0712F2BC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="3760" windowWidth="28800" windowHeight="12880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Data</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Der bringer ændringer i sin egen branch</t>
+  </si>
+  <si>
+    <t>Data2</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -368,7 +371,7 @@
     <col min="4" max="4" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,8 +387,11 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>123</v>
       </c>
@@ -401,20 +407,32 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F3">
         <v>2</v>
       </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F4">
         <v>3</v>
       </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F5">
         <v>4</v>
+      </c>
+      <c r="G5">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>